<commit_message>
time and vs upgrade
</commit_message>
<xml_diff>
--- a/Results/Results.xlsx
+++ b/Results/Results.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="l" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="l" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="k" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ly" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="op" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="l_1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ju" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -652,4 +657,1144 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tooth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Upper Value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upper Confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Central Value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Central Confidence</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Lower Value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Lower Confidence</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3_5,  ,  </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A3_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tooth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Upper Value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upper Confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Central Value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Central Confidence</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Lower Value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Lower Confidence</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3,  ,  </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A1,  ,  </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A3_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tooth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Upper Value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upper Confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Central Value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Central Confidence</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Lower Value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Lower Confidence</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3,  ,  </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A1,  ,  </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A3_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tooth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Upper Value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upper Confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Central Value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Central Confidence</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Lower Value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Lower Confidence</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3,  ,  </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3,  ,  </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A3_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Tooth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Upper Value</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Upper Confidence</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Central Value</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Central Confidence</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Lower Value</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Lower Confidence</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3,  ,  </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3_5,  ,  </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3,  ,  </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A3,  ,  </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A2,  ,  </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.1, 0.0, 0.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A3_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A4</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>B1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>B2</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>B3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>B4</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>C3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>C4</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>D4</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>